<commit_message>
Max Sub Array with Sum = k
</commit_message>
<xml_diff>
--- a/Coding Ninjas Sheet.xlsx
+++ b/Coding Ninjas Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Frontend\codingninjas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6004D830-72D9-45F7-B548-FE15FBCD1036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB0448-56D6-420C-8736-F0D0E76AA0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="5670" windowWidth="25800" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Path Sum</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/path-sum/</t>
+  </si>
+  <si>
+    <t>Path Sum II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-ii/submissions/</t>
   </si>
   <si>
     <r>
@@ -39,6 +45,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> sum exists or not in the tree
 </t>
@@ -49,6 +56,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Base Case : node == null return 
 Recurisve case : Recurse Left if not found then Right i.e left </t>
@@ -60,6 +68,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">OR </t>
     </r>
@@ -69,34 +78,40 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Right </t>
     </r>
+  </si>
+  <si>
+    <t>Maintain current path in a stack during the traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subarray-sum-equals-k/</t>
+  </si>
+  <si>
+    <t>Sub array sum == k</t>
+  </si>
+  <si>
+    <t>whenever sums has increased by a value of k, we've found a subarray of sums=k.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-iii/description/</t>
+  </si>
+  <si>
+    <t>Path Sum 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -106,16 +121,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,21 +173,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -358,39 +441,110 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="30.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.1796875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.81640625" style="2"/>
+    <col min="1" max="1" width="19.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.21875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="32.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:30" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="B2" s="8" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+    </row>
+    <row r="3" spans="1:30" s="2" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" s="2" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{7B616BEF-469C-464C-B0A9-CF2261712E62}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{5A3FA90E-9E98-4974-8225-92332095C7C8}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{8F645D6B-5B31-462A-82FA-6BF6DEABE21C}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{54D9C634-964F-4825-8B69-559203FC3F20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Remove Stars in a String
</commit_message>
<xml_diff>
--- a/Coding Ninjas Sheet.xlsx
+++ b/Coding Ninjas Sheet.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Frontend\codingninjas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8DB219-295F-4650-8840-109E4EB018DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE90568-ABF1-49C2-B0B2-A73C5E5494F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Easy one Shot" sheetId="1" r:id="rId1"/>
+    <sheet name="Time Taken" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Path Sum</t>
   </si>
@@ -348,13 +349,32 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1nw8GV8dOgiMQIy_v4-28SLCdvauwYhQa/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Minimum Depth of a Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-depth-of-binary-tree/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+maintain left and right sub tree values at every step if absent return inf, take min of them</t>
+  </si>
+  <si>
+    <t>2390. Removing Stars From a String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/removing-stars-from-a-string/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Stack </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -430,6 +450,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -514,7 +556,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -582,6 +624,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="3" builtinId="26"/>
@@ -806,12 +856,12 @@
   <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.21875" defaultRowHeight="51" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.21875" style="13"/>
+    <col min="1" max="1" width="39.88671875" style="13" customWidth="1"/>
     <col min="2" max="2" width="74.109375" style="13" customWidth="1"/>
     <col min="3" max="3" width="88" style="13" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="13" customWidth="1"/>
@@ -1113,6 +1163,17 @@
       <c r="AB10" s="21"/>
       <c r="AC10" s="21"/>
       <c r="AD10" s="21"/>
+    </row>
+    <row r="11" spans="1:35" s="25" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:35" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:35" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1170,8 +1231,45 @@
     <hyperlink ref="B6" r:id="rId7" xr:uid="{89A1C189-CC19-4415-85E2-A96D5B7E1030}"/>
     <hyperlink ref="B7" r:id="rId8" xr:uid="{C70C0E10-C118-457D-AFE3-340B9F5C2D24}"/>
     <hyperlink ref="B8" r:id="rId9" xr:uid="{605A7685-5234-4CA5-971D-DDB165CC132C}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{6BF29EE3-52DD-4A94-8604-9A3C11EC702F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2519D6AA-A3F0-46AD-A3F5-20A41B0B950B}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="65.77734375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="84.33203125" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A9971EF7-3693-45CD-B642-3F8B9110E54D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>